<commit_message>
database upload and storing completed
</commit_message>
<xml_diff>
--- a/data/database/CSE.xlsx
+++ b/data/database/CSE.xlsx
@@ -41,19 +41,19 @@
     <t>btech</t>
   </si>
   <si>
+    <t>Piyush Sharma</t>
+  </si>
+  <si>
+    <t>piyush@gmail.com</t>
+  </si>
+  <si>
+    <t>CSE</t>
+  </si>
+  <si>
     <t>Parth Gupta</t>
   </si>
   <si>
     <t>parth@gmail.com</t>
-  </si>
-  <si>
-    <t>CSE</t>
-  </si>
-  <si>
-    <t>Piyush Sharma</t>
-  </si>
-  <si>
-    <t>piyush@gmail.com</t>
   </si>
   <si>
     <t>Shaweta Choudhary</t>
@@ -170,7 +170,7 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -213,7 +213,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>12528</v>
+        <v>12502</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>8</v>
@@ -231,7 +231,7 @@
         <v>80</v>
       </c>
       <c r="H2" s="0" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -239,7 +239,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="n">
-        <v>12502</v>
+        <v>12528</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>11</v>
@@ -251,10 +251,10 @@
         <v>10</v>
       </c>
       <c r="F3" s="0" t="n">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="G3" s="0" t="n">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="H3" s="0" t="n">
         <v>9</v>
@@ -277,19 +277,19 @@
         <v>10</v>
       </c>
       <c r="F4" s="0" t="n">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="G4" s="0" t="n">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="H4" s="0" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" display="parth@gmail.com"/>
-    <hyperlink ref="D3" r:id="rId2" display="piyush@gmail.com"/>
+    <hyperlink ref="D2" r:id="rId1" display="piyush@gmail.com"/>
+    <hyperlink ref="D3" r:id="rId2" display="parth@gmail.com"/>
     <hyperlink ref="D4" r:id="rId3" display="shaweta@gmail.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
send invite - email
</commit_message>
<xml_diff>
--- a/data/database/CSE.xlsx
+++ b/data/database/CSE.xlsx
@@ -69,7 +69,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <name val="宋体"/>
@@ -90,13 +90,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <family val="2"/>
-      <charset val="134"/>
     </font>
   </fonts>
   <fills count="2">
@@ -141,12 +134,8 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -170,15 +159,15 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.3603238866397"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.668016194332"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.5748987854251"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.6599190283401"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.8097165991903"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="26.2388663967611"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.5748987854251"/>
   </cols>
   <sheetData>
@@ -208,7 +197,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>1</v>
       </c>
@@ -218,7 +207,7 @@
       <c r="C2" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="0" t="s">
         <v>9</v>
       </c>
       <c r="E2" s="0" t="s">
@@ -234,7 +223,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
         <v>2</v>
       </c>
@@ -244,7 +233,7 @@
       <c r="C3" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="0" t="s">
         <v>12</v>
       </c>
       <c r="E3" s="0" t="s">
@@ -260,7 +249,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
         <v>3</v>
       </c>
@@ -270,7 +259,7 @@
       <c r="C4" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="0" t="s">
         <v>14</v>
       </c>
       <c r="E4" s="0" t="s">
@@ -287,11 +276,6 @@
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" display="piyush@gmail.com"/>
-    <hyperlink ref="D3" r:id="rId2" display="parth@gmail.com"/>
-    <hyperlink ref="D4" r:id="rId3" display="shaweta@gmail.com"/>
-  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>